<commit_message>
Adição de arquivos de teste, atualização do .py principal
</commit_message>
<xml_diff>
--- a/GRARED_P.xlsx
+++ b/GRARED_P.xlsx
@@ -191,25 +191,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="justify" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="justify" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="justify" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -525,18 +525,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="1" customWidth="1"/>
+    <col min="2" max="3" width="8.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="6.85546875" style="5" customWidth="1"/>
     <col min="6" max="6" width="5.5703125" style="5" customWidth="1"/>
     <col min="7" max="7" width="8.42578125" style="1" customWidth="1"/>
@@ -558,7 +557,7 @@
     <col min="23" max="16384" width="15.7109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>5</v>
       </c>
@@ -567,37 +566,38 @@
       </c>
       <c r="C1" s="18"/>
       <c r="D1" s="15"/>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="12" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="13" t="s">
+      <c r="I1" s="13"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="13" t="s">
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="8"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
     </row>
-    <row r="2" spans="1:18" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>1</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>2</v>
       </c>
       <c r="D2" s="7">
@@ -621,7 +621,7 @@
       <c r="J2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="14"/>
+      <c r="K2" s="11"/>
       <c r="L2" s="3" t="s">
         <v>3</v>
       </c>
@@ -637,8 +637,9 @@
       <c r="P2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="8"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Correção de algumas falhas de arquivamenteo, e atualização de arquivos acessório
</commit_message>
<xml_diff>
--- a/GRARED_P.xlsx
+++ b/GRARED_P.xlsx
@@ -61,6 +61,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -91,7 +94,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -161,11 +164,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -230,6 +244,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,17 +548,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" style="1" customWidth="1"/>
-    <col min="2" max="3" width="8.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9" style="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="5" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" style="4" customWidth="1"/>
@@ -636,6 +654,51 @@
       <c r="O2" s="12"/>
       <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="24"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="24"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="24"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="24"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="24"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="24"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="24"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>